<commit_message>
Build Shared Medicine List
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/observation-norelevantfinding-1.xlsx
+++ b/output/SharedMedicinesList/observation-norelevantfinding-1.xlsx
@@ -701,9 +701,6 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -719,9 +716,6 @@
     <t>An observation exists to have a value, though it may not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">type:$this}
 </t>
   </si>
@@ -748,7 +742,13 @@
     <t>363714003 |Interprets|</t>
   </si>
   <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
     <t>Coded value of the observation</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/assertion-of-absence-1</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -3849,9 +3849,7 @@
       <c r="A21" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="B21" t="s" s="2">
-        <v>217</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>45</v>
       </c>
@@ -3863,7 +3861,7 @@
         <v>56</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>45</v>
@@ -3875,16 +3873,16 @@
         <v>142</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3909,24 +3907,26 @@
         <v>45</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X21" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y21" t="s" s="2">
-        <v>222</v>
+        <v>45</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AE21" t="s" s="2">
         <v>216</v>
@@ -3938,36 +3938,36 @@
         <v>56</v>
       </c>
       <c r="AH21" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK21" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL21" t="s" s="2">
+      <c r="AN21" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO21" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="AM21" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>230</v>
-      </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>216</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>45</v>
@@ -3980,7 +3980,7 @@
         <v>56</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>45</v>
@@ -3992,16 +3992,16 @@
         <v>142</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L22" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4026,11 +4026,11 @@
         <v>45</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4057,28 +4057,28 @@
         <v>56</v>
       </c>
       <c r="AH22" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AI22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO22" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>230</v>
       </c>
     </row>
     <row r="23" hidden="true">
@@ -4182,7 +4182,7 @@
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
@@ -7390,13 +7390,13 @@
         <v>395</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>396</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7466,16 +7466,16 @@
         <v>397</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO51" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>230</v>
       </c>
     </row>
     <row r="52" hidden="true">

</xml_diff>

<commit_message>
Regenerated SML IG outputs - various improvements, including:
- updated HL7 AU STU3 dependency to v1.1.1
- improvements to links for a number of examples
- improvements to intro descriptions of 2 profiles
- MHR patient profile; updated status to 'active' and experimental to 'false'; improved profile description and description of invariant
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/observation-norelevantfinding-1.xlsx
+++ b/output/SharedMedicinesList/observation-norelevantfinding-1.xlsx
@@ -166,7 +166,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or code!=component.code}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}inv-dh-obs-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-obs-02:If present, a performer shall at least have a reference, an identifier or a display {performer.exists() implies performer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}obs-7:If code is the same as a component code then the value element associated with the code SHALL NOT be present {value.empty() or component.code.where( (coding.code = %resource.code.coding.code) and (coding.system = %resource.code.coding.system)).empty()}obs-6:dataAbsentReason SHALL only be present if Observation.value[x] is not present {dataAbsentReason.empty() or value.empty()}inv-dh-obs-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-obs-02:If present, a performer shall at least have a reference, an identifier or a display {performer.exists() implies performer.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
   </si>
   <si>
     <t>Event</t>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>56</v>

</xml_diff>